<commit_message>
correçoes e inicio da automatizacao
</commit_message>
<xml_diff>
--- a/src/data/func.xlsx
+++ b/src/data/func.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniel Costa\OneDrive\Desktop\GitHubProjetos\AutomForm\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniel Costa\OneDrive\Desktop\GitHubProjetos\AutomForm\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21D49D-694B-4FA8-A687-1237CAC1720D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F822F225-DFF6-4FB3-B459-9205C27B4CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="557" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>BAIRRO</t>
   </si>
   <si>
-    <t>ESTADO</t>
-  </si>
-  <si>
     <t>CEP</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>BOM JESUS</t>
+  </si>
+  <si>
+    <t>UF</t>
   </si>
 </sst>
 </file>
@@ -349,22 +349,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -400,6 +391,182 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFE3E3E3"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFE3E3E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFE3E3E3"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFE3E3E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="000"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color rgb="FFE3E3E3"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFE3E3E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFE3E3E3"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFE3E3E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFE3E3E3"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="medium">
+          <color rgb="FFE3E3E3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.6"/>
+        <color auto="1"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -499,182 +666,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="000"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color rgb="FFE3E3E3"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFE3E3E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFE3E3E3"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFE3E3E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFE3E3E3"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFE3E3E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFE3E3E3"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFE3E3E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFE3E3E3"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="medium">
-          <color rgb="FFE3E3E3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9.6"/>
-        <color auto="1"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -963,8 +954,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98170362-954E-463D-97A6-DB0349485094}" name="Tabela1" displayName="Tabela1" ref="A1:N16" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
-  <autoFilter ref="A1:N16" xr:uid="{98170362-954E-463D-97A6-DB0349485094}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{98170362-954E-463D-97A6-DB0349485094}" name="Tabela1" displayName="Tabela1" ref="A1:N12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+  <autoFilter ref="A1:N12" xr:uid="{98170362-954E-463D-97A6-DB0349485094}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{20EE5067-D5D3-4EAD-9D13-184E4E0E30E9}" name="MATRICULA" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{781A80EC-4BDE-4771-BBAB-D510650C39CD}" name="NOME" dataDxfId="12"/>
@@ -974,12 +965,12 @@
     <tableColumn id="8" xr3:uid="{2D63EF05-502E-4255-90E0-0181E37416E7}" name="NUMERO" dataDxfId="8"/>
     <tableColumn id="9" xr3:uid="{672D5914-C4F1-4806-82F6-689560AB1AB9}" name="COMPLEMENTO" dataDxfId="7"/>
     <tableColumn id="10" xr3:uid="{5FFA608E-F4AD-4296-882A-846BB9364503}" name="BAIRRO" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{DE860180-AEAE-4992-B37E-807BD2F0B6A9}" name="MUNICIPIO" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{07645448-A6E5-4C25-8C71-D21E37AF06CD}" name="ESTADO" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{7F6235CC-3F3C-40F7-B48E-869369C047D0}" name="CEP" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{444622AC-0155-44D9-9152-DCB64822E898}" name="DDD" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{99F5131E-2A4F-41D3-B749-C22A6354761B}" name="CELULAR" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{EEEED4E4-987A-41C7-B0E6-DD3D7D0FDF09}" name="FONE" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{DE860180-AEAE-4992-B37E-807BD2F0B6A9}" name="MUNICIPIO" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{07645448-A6E5-4C25-8C71-D21E37AF06CD}" name="UF" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{7F6235CC-3F3C-40F7-B48E-869369C047D0}" name="CEP" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{444622AC-0155-44D9-9152-DCB64822E898}" name="DDD" dataDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{99F5131E-2A4F-41D3-B749-C22A6354761B}" name="CELULAR" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{EEEED4E4-987A-41C7-B0E6-DD3D7D0FDF09}" name="FONE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1248,13 +1239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,7 +1265,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1292,571 +1283,507 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="I2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="3">
         <v>12345678</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="3">
         <v>11</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="3">
         <v>987654321</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="3">
         <v>98765432</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="3">
+        <v>98765432100</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6">
-        <v>98765432100</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="I3" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="3">
         <v>54321098</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="3">
         <v>21</v>
       </c>
-      <c r="M3" s="6">
+      <c r="M3" s="3">
         <v>987654321</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>19</v>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="3">
+        <v>45678912300</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="6">
-        <v>45678912300</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K4" s="6">
+      <c r="I4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="3">
         <v>98765432</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="3">
         <v>31</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="3">
         <v>987654321</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="3">
         <v>98765432</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3">
+        <v>78912345600</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="6">
-        <v>78912345600</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="I5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="3">
         <v>34567890</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="3">
         <v>71</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="3">
         <v>987654321</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>19</v>
+      <c r="N5" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3">
+        <v>23456789000</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="6">
-        <v>23456789000</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="6">
+      <c r="I6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="3">
         <v>67890123</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="3">
         <v>81</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="3">
         <v>987654321</v>
       </c>
-      <c r="N6" s="6" t="s">
-        <v>19</v>
+      <c r="N6" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3">
+        <v>67890123400</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="6">
-        <v>67890123400</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="F7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="I7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="3">
         <v>90123456</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="3">
         <v>51</v>
       </c>
-      <c r="M7" s="6">
+      <c r="M7" s="3">
         <v>987654321</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>19</v>
+      <c r="N7" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="3">
+        <v>34567890100</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="6">
-        <v>34567890100</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="I8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="3">
         <v>23456789</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="3">
         <v>85</v>
       </c>
-      <c r="M8" s="6">
+      <c r="M8" s="3">
         <v>987654321</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="3">
         <v>98765432</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="3">
+        <v>90123456700</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="6">
-        <v>90123456700</v>
-      </c>
-      <c r="E9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="K9" s="6">
+      <c r="I9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="K9" s="3">
         <v>56789012</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="3">
         <v>41</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="3">
         <v>987654321</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>19</v>
+      <c r="N9" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="3">
+        <v>56789012300</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="6">
-        <v>56789012300</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="6">
+      <c r="I10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="3">
         <v>89012345</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="3">
         <v>92</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="3">
         <v>987654321</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="3">
         <v>98765432</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12345678900</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="F11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="4">
+        <v>45678901</v>
+      </c>
+      <c r="L11" s="4">
         <v>61</v>
       </c>
-      <c r="D11" s="7">
-        <v>12345678900</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="7">
-        <v>45678901</v>
-      </c>
-      <c r="L11" s="7">
-        <v>61</v>
-      </c>
-      <c r="M11" s="7">
+      <c r="M11" s="4">
         <v>987654321</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="4">
         <v>98765432</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="K12" s="6">
+      <c r="I12" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="3">
         <v>56789012</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="4">
         <v>83</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>983321492</v>
       </c>
-      <c r="N12" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="N12" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
correcoes na parte de municipios
</commit_message>
<xml_diff>
--- a/src/data/func.xlsx
+++ b/src/data/func.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haniel Costa\OneDrive\Desktop\GitHubProjetos\AutomForm\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F822F225-DFF6-4FB3-B459-9205C27B4CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35FD1E83-1E69-4C2B-B3E4-8903F1710974}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="557" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1245,7 +1245,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,90 +1347,90 @@
     </row>
     <row r="3" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D3" s="3">
-        <v>98765432100</v>
+        <v>45678912300</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K3" s="3">
-        <v>54321098</v>
+        <v>98765432</v>
       </c>
       <c r="L3" s="3">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M3" s="3">
         <v>987654321</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>18</v>
+      <c r="N3" s="3">
+        <v>98765432</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D4" s="3">
-        <v>45678912300</v>
+        <v>98765432100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K4" s="3">
-        <v>98765432</v>
+        <v>54321098</v>
       </c>
       <c r="L4" s="3">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="M4" s="3">
         <v>987654321</v>
       </c>
-      <c r="N4" s="3">
-        <v>98765432</v>
+      <c r="N4" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>